<commit_message>
Atualizar nome da planilha para Palavras-chave e reduzir tempo de espera na análise de resultados
</commit_message>
<xml_diff>
--- a/Resultado_Automacao_Belgo.xlsx
+++ b/Resultado_Automacao_Belgo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,881 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Patrocinado Belgo e Concorrente</t>
+          <t>Outros</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cordoalha belgo 7 fios 500 metros</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Patrocinado Belgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>arame farpado belgo motto 500m</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>arame farpado belgo rodeio 500m</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>arame fortte 500m</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>belgo campestre carneiro</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>poste belgo</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>tela galinheiro belgo</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>arame farpado belgo 500m</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>arame fruticultura belgo frutifio 1000m</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>concertina belgo</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>portão belgo</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>tela carneiro belgo</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>arame belgo 500 metros</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>arame farpado fortte belgo 500m</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>arames lisos para cerca</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>tela alambrado belgo</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>tela pinteiro belgo</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>tela soldada belgo tabela</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>belgo bekaert arames</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>arame motto 500m</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C25" t="n">
+        <v>29</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>grampo belgo</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>arame farpado motto 500 metros</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C27" t="n">
+        <v>15</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>arame rodeio 500m</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C28" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>arame farpado fortte rolo 500m</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>arame farpado rodeio 500m</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>cordoalha para curral 7 fios 500 metros belgo</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>arame liso para cerca z700</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>arame farpado 500m belgo</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>belgo arames</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="C34" t="n">
+        <v>15</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>arame liso belgo fortte 1000m</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="C35" t="n">
+        <v>11</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>tela campestre carneiro</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>arame liso belgo z 700 rolo de 1000 metros</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>arame farpado 500m motto</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C38" t="n">
+        <v>14</v>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>arame z700 belgo 1000 metros</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cordoalha para curral 7 fios belgo</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C40" t="n">
+        <v>7</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>belgo eletrix 1000m</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>tela carneiro</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>arame farpado moto</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="C43" t="n">
+        <v>6</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>arame liso z 700</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="C44" t="n">
+        <v>6</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>arame belgo eletrix 1000m</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="C45" t="n">
+        <v>3</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>arame belgo</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>cerca pronta belgo campestre carneiro</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>arame farpado motto</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C48" t="n">
+        <v>19</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>arame eletrix 1000m</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C49" t="n">
+        <v>3</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>tela mangueirão belgo</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>arame farpado motto 500m</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="C51" t="n">
+        <v>7</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Orgânico Belgo e Concorrente</t>
         </is>
       </c>
     </row>

</xml_diff>